<commit_message>
light controller destroy bug fixed
</commit_message>
<xml_diff>
--- a/간트차트.xlsx
+++ b/간트차트.xlsx
@@ -946,28 +946,28 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="30" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="5" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - 강조색5" xfId="4" builtinId="46"/>
@@ -1358,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1384,73 +1384,73 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="V5" s="52"/>
-      <c r="W5" s="52"/>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="53"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="56"/>
+      <c r="H5" s="56"/>
+      <c r="I5" s="56"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="56"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="56"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="56"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="57"/>
     </row>
     <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="49"/>
-      <c r="C6" s="51" t="s">
+      <c r="B6" s="53"/>
+      <c r="C6" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="51" t="s">
+      <c r="D6" s="57"/>
+      <c r="E6" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="51" t="s">
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="53"/>
-      <c r="O6" s="51" t="s">
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="51" t="s">
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="52"/>
-      <c r="V6" s="52"/>
-      <c r="W6" s="52"/>
-      <c r="X6" s="52"/>
-      <c r="Y6" s="53"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56"/>
+      <c r="Y6" s="57"/>
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="50"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="36">
         <v>44133</v>
       </c>
@@ -2117,13 +2117,13 @@
       <c r="A3" s="34">
         <v>11.02</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="50" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="34">
         <v>11.04</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="48" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2131,13 +2131,13 @@
       <c r="A4" s="34">
         <v>11.03</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="51" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="34">
         <v>11.05</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="48" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2145,13 +2145,13 @@
       <c r="A5" s="34">
         <v>11.05</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="51" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="34">
         <v>11.05</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="49" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2161,7 +2161,7 @@
       <c r="C6" s="34">
         <v>11.06</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="49" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Camera connect & image pop-up done! (GDI+ so might be problem with future features but good luck....!
</commit_message>
<xml_diff>
--- a/간트차트.xlsx
+++ b/간트차트.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="간트" sheetId="1" r:id="rId1"/>
     <sheet name="주석" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -195,11 +195,11 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>2. 영상 획득은 문제가 없으나, Picture Control 시현이 불가능함 현재는..</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
     <t>5. 2번 Cimage로 하려다 안돼서 GDIPlus 활용 예정. 개발중</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. GDIPlus bitmap access violation……………….. 어디가 문제지..</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -210,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm\.dd"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +346,16 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,8 +394,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -832,8 +845,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
@@ -850,8 +872,11 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -950,6 +975,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="31" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="5" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="31" xfId="6" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -968,9 +994,17 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="20% - 강조색5" xfId="4" builtinId="46"/>
+    <cellStyle name="나쁨" xfId="6" builtinId="27"/>
     <cellStyle name="메모" xfId="2" builtinId="10"/>
     <cellStyle name="보통" xfId="5" builtinId="28"/>
     <cellStyle name="입력" xfId="3" builtinId="20"/>
@@ -1358,9 +1392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1384,73 +1416,73 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="56"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="57"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
+      <c r="Y5" s="58"/>
     </row>
     <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="53"/>
-      <c r="C6" s="55" t="s">
+      <c r="B6" s="54"/>
+      <c r="C6" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="55" t="s">
+      <c r="D6" s="58"/>
+      <c r="E6" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="55" t="s">
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="55" t="s">
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="55" t="s">
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
+      <c r="R6" s="57"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="V6" s="57"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
+      <c r="Y6" s="58"/>
     </row>
     <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="54"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="36">
         <v>44133</v>
       </c>
@@ -2073,7 +2105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2121,10 +2153,10 @@
         <v>30</v>
       </c>
       <c r="C3" s="34">
-        <v>11.04</v>
+        <v>11.05</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2137,8 +2169,8 @@
       <c r="C4" s="34">
         <v>11.05</v>
       </c>
-      <c r="D4" s="48" t="s">
-        <v>37</v>
+      <c r="D4" s="49" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2149,32 +2181,32 @@
         <v>38</v>
       </c>
       <c r="C5" s="34">
-        <v>11.05</v>
+        <v>11.06</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" s="29"/>
-      <c r="C6" s="34">
+      <c r="C6" s="59">
         <v>11.06</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="52" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="34"/>
       <c r="B7" s="29"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="30"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="60"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="34"/>
       <c r="B8" s="29"/>
-      <c r="C8" s="34"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>